<commit_message>
Más cambios en la Base de Datos
</commit_message>
<xml_diff>
--- a/Base de Datos/COMPUTACIÓN 201835  Semestral.xlsx
+++ b/Base de Datos/COMPUTACIÓN 201835  Semestral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTO_SCRUM_IS_II\LoboServicesFCC\Base de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5182C2BB-F736-4073-99BF-A57BFA254044}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B8C93D-B3C0-42B9-807F-4B64E6FB5808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3611" uniqueCount="1268">
   <si>
     <t>BENEMÉRITA UNIVERSIDAD AUTÓNOMA DE PUEBLA</t>
   </si>
@@ -3658,6 +3658,189 @@
   </si>
   <si>
     <t>Lengua Extranjera III</t>
+  </si>
+  <si>
+    <t>Ecuaciones Diferenciales</t>
+  </si>
+  <si>
+    <t>Circuitos Eléctricos</t>
+  </si>
+  <si>
+    <t>Graficación</t>
+  </si>
+  <si>
+    <t>Estructura de Datos</t>
+  </si>
+  <si>
+    <t>Lengua Extranjera IV</t>
+  </si>
+  <si>
+    <t>Probabilidad y Estadística</t>
+  </si>
+  <si>
+    <t>Circuitos Electrónicos</t>
+  </si>
+  <si>
+    <t>Sistemas Operativos I</t>
+  </si>
+  <si>
+    <t>Análisis y Diseño de Algoritmos</t>
+  </si>
+  <si>
+    <t>Ingeniería de Software</t>
+  </si>
+  <si>
+    <t>Modelos de Redes</t>
+  </si>
+  <si>
+    <t>Diseño Digital</t>
+  </si>
+  <si>
+    <t>Bases de Datos para Ingeniería</t>
+  </si>
+  <si>
+    <t>Sistemas Operativos II</t>
+  </si>
+  <si>
+    <t>Administración de Proyectos</t>
+  </si>
+  <si>
+    <t>Redes Inalámbricas</t>
+  </si>
+  <si>
+    <t>Minería de Datos</t>
+  </si>
+  <si>
+    <t>Arquitectura de Cómputo</t>
+  </si>
+  <si>
+    <t>Programación Recurrente y Paralela</t>
+  </si>
+  <si>
+    <t>Desarrollo de Aplicaciones Web</t>
+  </si>
+  <si>
+    <t>Teoría de Control</t>
+  </si>
+  <si>
+    <t>Administración de Redes</t>
+  </si>
+  <si>
+    <t>Técnicas de Inteligencia Artificial</t>
+  </si>
+  <si>
+    <t>Programación Distribuida Aplicada</t>
+  </si>
+  <si>
+    <t>Desarrollo de Aplicaciones Móviles</t>
+  </si>
+  <si>
+    <t>OptativaI</t>
+  </si>
+  <si>
+    <t>OptativaII</t>
+  </si>
+  <si>
+    <t>OptativaDESIT</t>
+  </si>
+  <si>
+    <t>Métodos Numéricos</t>
+  </si>
+  <si>
+    <t>Máquinas de Aprendizaje</t>
+  </si>
+  <si>
+    <t>Lógica Matemática</t>
+  </si>
+  <si>
+    <t>Lenguajes de Programación</t>
+  </si>
+  <si>
+    <t>Interacción Humano Computadora</t>
+  </si>
+  <si>
+    <t>Intercomunicación y Seguridad en Redes</t>
+  </si>
+  <si>
+    <t>Sistemas Empotrados</t>
+  </si>
+  <si>
+    <t>Servicio Social</t>
+  </si>
+  <si>
+    <t>Procesamiento Digital de Imágenes</t>
+  </si>
+  <si>
+    <t>Tratamiento de la Información</t>
+  </si>
+  <si>
+    <t>Recuperación de la Información</t>
+  </si>
+  <si>
+    <t>Simulación</t>
+  </si>
+  <si>
+    <t>Cómputo Ubicuo</t>
+  </si>
+  <si>
+    <t>Arquitectura Avanzada de Computadoras</t>
+  </si>
+  <si>
+    <t>Investigación de Operaciones</t>
+  </si>
+  <si>
+    <t>Súper Cómputo</t>
+  </si>
+  <si>
+    <t>Sistemas Interactivos Modernos</t>
+  </si>
+  <si>
+    <t>Web Semántico</t>
+  </si>
+  <si>
+    <t>Almacenamiento de Datos</t>
+  </si>
+  <si>
+    <t>Control Digital</t>
+  </si>
+  <si>
+    <t>Robótica Aplicada</t>
+  </si>
+  <si>
+    <t>Reconocimiento de Patrones</t>
+  </si>
+  <si>
+    <t>Sistemas en Tiempo Real</t>
+  </si>
+  <si>
+    <t>Visión y Animación por Computadora</t>
+  </si>
+  <si>
+    <t>Práctica Profesional</t>
+  </si>
+  <si>
+    <t>Proyecto I + D I</t>
+  </si>
+  <si>
+    <t>Animación por Computadora</t>
+  </si>
+  <si>
+    <t>Aplicaciones Multimedia</t>
+  </si>
+  <si>
+    <t>Aplicaciones Web</t>
+  </si>
+  <si>
+    <t>idMateria1</t>
+  </si>
+  <si>
+    <t>idMateria2</t>
+  </si>
+  <si>
+    <t>Ingeniería de Software Avanzada</t>
+  </si>
+  <si>
+    <t>Introducción a los Compiladores</t>
   </si>
 </sst>
 </file>
@@ -21083,20 +21266,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03379B5D-3AFA-44CA-B431-D65A6289F440}">
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" customWidth="1"/>
     <col min="4" max="4" width="8.77734375" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>1188</v>
       </c>
@@ -21106,127 +21291,1847 @@
       <c r="D2" s="4" t="s">
         <v>1189</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="4" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>1233</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>1264</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
       <c r="C3" t="s">
         <v>1190</v>
       </c>
       <c r="D3" s="2">
         <v>6</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
       <c r="C4" t="s">
         <v>1191</v>
       </c>
       <c r="D4" s="2">
         <v>6</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
       <c r="C5" t="s">
         <v>1192</v>
       </c>
       <c r="D5" s="2">
         <v>4</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
       <c r="C6" t="s">
         <v>1193</v>
       </c>
       <c r="D6" s="2">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
       <c r="C7" t="s">
         <v>1194</v>
       </c>
       <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
       <c r="C8" t="s">
         <v>1195</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D8" s="2">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>6</v>
+      </c>
+      <c r="J8" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
       <c r="C9" t="s">
         <v>1196</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="2">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>7</v>
+      </c>
+      <c r="J9" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
       <c r="C10" t="s">
         <v>1197</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D10" s="2">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>8</v>
+      </c>
+      <c r="J10" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>9</v>
+      </c>
       <c r="C11" t="s">
         <v>1198</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D11" s="2">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
       <c r="C12" t="s">
         <v>1199</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D12" s="2">
+        <v>4</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>9</v>
+      </c>
+      <c r="J12" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
+        <v>11</v>
+      </c>
       <c r="C13" t="s">
         <v>1200</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D13" s="2">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>9</v>
+      </c>
+      <c r="J13" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
+        <v>12</v>
+      </c>
       <c r="C14" t="s">
         <v>1201</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D14" s="2">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>10</v>
+      </c>
+      <c r="J14" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
+        <v>13</v>
+      </c>
       <c r="C15" t="s">
         <v>1202</v>
       </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D15" s="2">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>12</v>
+      </c>
+      <c r="J15" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
+        <v>14</v>
+      </c>
       <c r="C16" t="s">
         <v>1203</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="2">
+        <v>6</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>12</v>
+      </c>
+      <c r="J16" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="2">
+        <v>15</v>
+      </c>
       <c r="C17" t="s">
         <v>1204</v>
       </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="2">
+        <v>6</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>13</v>
+      </c>
+      <c r="J17" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
+        <v>16</v>
+      </c>
       <c r="C18" t="s">
         <v>1205</v>
       </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="2">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>15</v>
+      </c>
+      <c r="J18" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
+        <v>17</v>
+      </c>
       <c r="C19" t="s">
         <v>1206</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2">
+        <v>4</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <v>15</v>
+      </c>
+      <c r="J19" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D20" s="2">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <v>15</v>
+      </c>
+      <c r="J20" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="2">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D21" s="2">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <v>16</v>
+      </c>
+      <c r="J21" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D22" s="2">
+        <v>6</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>17</v>
+      </c>
+      <c r="J22" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D23" s="2">
+        <v>6</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>18</v>
+      </c>
+      <c r="J23" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <v>19</v>
+      </c>
+      <c r="J24" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="2">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D25" s="2">
+        <v>6</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <v>21</v>
+      </c>
+      <c r="J25" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="2">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D26" s="2">
+        <v>6</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>21</v>
+      </c>
+      <c r="J26" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D27" s="2">
+        <v>6</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>21</v>
+      </c>
+      <c r="J27" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="2">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D28" s="2">
+        <v>6</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>23</v>
+      </c>
+      <c r="J28" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="2">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D29" s="2">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <v>23</v>
+      </c>
+      <c r="J29" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="2">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D30" s="2">
+        <v>6</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2">
+        <v>24</v>
+      </c>
+      <c r="J30" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="2">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D31" s="2">
+        <v>6</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>25</v>
+      </c>
+      <c r="J31" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="2">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D32" s="2">
+        <v>6</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <v>26</v>
+      </c>
+      <c r="J32" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="2">
+        <v>31</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D33" s="2">
+        <v>6</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <v>26</v>
+      </c>
+      <c r="J33" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B34" s="2">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D34" s="2">
+        <v>5</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <v>28</v>
+      </c>
+      <c r="J34" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B35" s="2">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D35" s="2">
+        <v>6</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2">
+        <v>29</v>
+      </c>
+      <c r="J35" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="2">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D36" s="2">
+        <v>6</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+      <c r="I36" s="2">
+        <v>32</v>
+      </c>
+      <c r="J36" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="2">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D37" s="2">
+        <v>6</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0</v>
+      </c>
+      <c r="I37" s="2">
+        <v>32</v>
+      </c>
+      <c r="J37" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="2">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D38" s="2">
+        <v>6</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0</v>
+      </c>
+      <c r="I38" s="2">
+        <v>33</v>
+      </c>
+      <c r="J38" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="2">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D39" s="2">
+        <v>6</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0</v>
+      </c>
+      <c r="I39" s="2">
+        <v>35</v>
+      </c>
+      <c r="J39" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="2">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D40" s="2">
+        <v>6</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <v>36</v>
+      </c>
+      <c r="J40" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="2">
+        <v>39</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D41" s="2">
+        <v>6</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0</v>
+      </c>
+      <c r="I41" s="2">
+        <v>37</v>
+      </c>
+      <c r="J41" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="2">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D42" s="2">
+        <v>6</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2">
+        <v>39</v>
+      </c>
+      <c r="J42" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="2">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D43" s="2">
+        <v>6</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2">
+        <v>18</v>
+      </c>
+      <c r="J43" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="2">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D44" s="2">
+        <v>6</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2">
+        <v>34</v>
+      </c>
+      <c r="J44" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B45" s="2">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D45" s="2">
+        <v>6</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2">
+        <v>14</v>
+      </c>
+      <c r="J45" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B46" s="2">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D46" s="2">
+        <v>6</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0</v>
+      </c>
+      <c r="I46" s="2">
+        <v>26</v>
+      </c>
+      <c r="J46" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B47" s="2">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D47" s="2">
+        <v>6</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0</v>
+      </c>
+      <c r="I47" s="2">
+        <v>27</v>
+      </c>
+      <c r="J47" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B48" s="2">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D48" s="2">
+        <v>6</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2">
+        <v>27</v>
+      </c>
+      <c r="J48" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B49" s="2">
+        <v>47</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D49" s="2">
+        <v>6</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0</v>
+      </c>
+      <c r="I49" s="2">
+        <v>20</v>
+      </c>
+      <c r="J49" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B50" s="2">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D50" s="2">
+        <v>6</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0</v>
+      </c>
+      <c r="I50" s="2">
+        <v>21</v>
+      </c>
+      <c r="J50" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B51" s="2">
+        <v>49</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D51" s="2">
+        <v>6</v>
+      </c>
+      <c r="E51" s="2">
+        <v>1</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0</v>
+      </c>
+      <c r="G51" s="2">
+        <v>0</v>
+      </c>
+      <c r="I51" s="2">
+        <v>30</v>
+      </c>
+      <c r="J51" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B52" s="2">
+        <v>50</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D52" s="2">
+        <v>6</v>
+      </c>
+      <c r="E52" s="2">
+        <v>1</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0</v>
+      </c>
+      <c r="I52" s="2">
+        <v>30</v>
+      </c>
+      <c r="J52" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B53" s="2">
+        <v>51</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D53" s="2">
+        <v>6</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0</v>
+      </c>
+      <c r="G53" s="2">
+        <v>0</v>
+      </c>
+      <c r="I53" s="2">
+        <v>23</v>
+      </c>
+      <c r="J53" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B54" s="2">
+        <v>52</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D54" s="2">
+        <v>6</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0</v>
+      </c>
+      <c r="G54" s="2">
+        <v>0</v>
+      </c>
+      <c r="I54" s="2">
+        <v>37</v>
+      </c>
+      <c r="J54" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B55" s="2">
+        <v>53</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D55" s="2">
+        <v>6</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0</v>
+      </c>
+      <c r="I55" s="2">
+        <v>35</v>
+      </c>
+      <c r="J55" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B56" s="2">
+        <v>54</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D56" s="2">
+        <v>6</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2">
+        <v>43</v>
+      </c>
+      <c r="J56" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B57" s="2">
+        <v>55</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D57" s="2">
+        <v>6</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0</v>
+      </c>
+      <c r="G57" s="2">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2">
+        <v>46</v>
+      </c>
+      <c r="J57" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B58" s="2">
+        <v>56</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D58" s="2">
+        <v>6</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2">
+        <v>46</v>
+      </c>
+      <c r="J58" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B59" s="2">
+        <v>57</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D59" s="2">
+        <v>10</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0</v>
+      </c>
+      <c r="G59" s="2">
+        <v>0</v>
+      </c>
+      <c r="I59" s="2">
+        <v>34</v>
+      </c>
+      <c r="J59" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B60" s="2">
+        <v>58</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D60" s="2">
+        <v>6</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0</v>
+      </c>
+      <c r="F60" s="2">
+        <v>1</v>
+      </c>
+      <c r="G60" s="2">
+        <v>0</v>
+      </c>
+      <c r="I60" s="2">
+        <v>34</v>
+      </c>
+      <c r="J60" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B61" s="2">
+        <v>59</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D61" s="2">
+        <v>6</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0</v>
+      </c>
+      <c r="F61" s="2">
+        <v>1</v>
+      </c>
+      <c r="G61" s="2">
+        <v>0</v>
+      </c>
+      <c r="I61" s="2">
+        <v>38</v>
+      </c>
+      <c r="J61" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B62" s="2">
+        <v>60</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D62" s="2">
+        <v>6</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0</v>
+      </c>
+      <c r="F62" s="2">
+        <v>1</v>
+      </c>
+      <c r="G62" s="2">
+        <v>0</v>
+      </c>
+      <c r="I62" s="2">
+        <v>40</v>
+      </c>
+      <c r="J62" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B63" s="2">
+        <v>61</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D63" s="2">
+        <v>6</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0</v>
+      </c>
+      <c r="F63" s="2">
+        <v>1</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0</v>
+      </c>
+      <c r="I63" s="2">
+        <v>44</v>
+      </c>
+      <c r="J63" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B64" s="2">
+        <v>62</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D64" s="2">
+        <v>6</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0</v>
+      </c>
+      <c r="F64" s="2">
+        <v>1</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B65" s="2">
+        <v>63</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D65" s="2">
+        <v>6</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0</v>
+      </c>
+      <c r="F65" s="2">
+        <v>1</v>
+      </c>
+      <c r="G65" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B66" s="2">
+        <v>64</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D66" s="2">
+        <v>6</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1</v>
+      </c>
+      <c r="G66" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B67" s="2">
+        <v>65</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D67" s="2">
+        <v>6</v>
+      </c>
+      <c r="E67" s="2">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2">
+        <v>1</v>
+      </c>
+      <c r="G67" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B68" s="2">
+        <v>66</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D68" s="2">
+        <v>6</v>
+      </c>
+      <c r="E68" s="2">
+        <v>0</v>
+      </c>
+      <c r="F68" s="2">
+        <v>1</v>
+      </c>
+      <c r="G68" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B69" s="2">
+        <v>67</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D69" s="2">
+        <v>6</v>
+      </c>
+      <c r="E69" s="2">
+        <v>0</v>
+      </c>
+      <c r="F69" s="2">
+        <v>1</v>
+      </c>
+      <c r="G69" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B70" s="2">
+        <v>68</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D70" s="2">
+        <v>6</v>
+      </c>
+      <c r="E70" s="2">
+        <v>0</v>
+      </c>
+      <c r="F70" s="2">
+        <v>1</v>
+      </c>
+      <c r="G70" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B71" s="2">
+        <v>69</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D71" s="2">
+        <v>5</v>
+      </c>
+      <c r="E71" s="2">
+        <v>0</v>
+      </c>
+      <c r="F71" s="2">
+        <v>0</v>
+      </c>
+      <c r="G71" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B72" s="2">
+        <v>70</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D72" s="2">
+        <v>5</v>
+      </c>
+      <c r="E72" s="2">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2">
+        <v>0</v>
+      </c>
+      <c r="G72" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B73" s="2">
+        <v>71</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D73" s="2">
+        <v>5</v>
+      </c>
+      <c r="E73" s="2">
+        <v>0</v>
+      </c>
+      <c r="F73" s="2">
+        <v>0</v>
+      </c>
+      <c r="G73" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B74" s="2">
+        <v>72</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D74" s="2">
+        <v>5</v>
+      </c>
+      <c r="E74" s="2">
+        <v>0</v>
+      </c>
+      <c r="F74" s="2">
+        <v>0</v>
+      </c>
+      <c r="G74" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B75" s="2">
+        <v>73</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D75" s="2">
+        <v>5</v>
+      </c>
+      <c r="E75" s="2">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2">
+        <v>0</v>
+      </c>
+      <c r="G75" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se empezo lo de graficas
</commit_message>
<xml_diff>
--- a/Base de Datos/COMPUTACIÓN 201835  Semestral.xlsx
+++ b/Base de Datos/COMPUTACIÓN 201835  Semestral.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTO_SCRUM_IS_II\LoboServicesFCC\Base de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B5DFFA-CC42-488D-ADA7-187C0983E6BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D8253B-5B05-4122-A80C-EA7FD9083CBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="semestral" sheetId="6" r:id="rId1"/>
-    <sheet name="cargarmaterias" sheetId="14" r:id="rId2"/>
+    <sheet name="maestro(admin)" sheetId="14" r:id="rId2"/>
     <sheet name="materias" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3611" uniqueCount="1268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3616" uniqueCount="1271">
   <si>
     <t>BENEMÉRITA UNIVERSIDAD AUTÓNOMA DE PUEBLA</t>
   </si>
@@ -3842,6 +3842,15 @@
   </si>
   <si>
     <t>Introducción a los Compiladores</t>
+  </si>
+  <si>
+    <t>matricula</t>
+  </si>
+  <si>
+    <t>contrasena</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -4760,7 +4769,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D1181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1110" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A1122" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F1154" sqref="F1154"/>
     </sheetView>
   </sheetViews>
@@ -21277,14 +21286,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82DFC6E-E826-4178-AF7A-7971C314C365}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -21293,7 +21325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03379B5D-3AFA-44CA-B431-D65A6289F440}">
   <dimension ref="B2:J75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Mejoras en la historia de ver ocupacion materias
</commit_message>
<xml_diff>
--- a/Base de Datos/COMPUTACIÓN 201835  Semestral.xlsx
+++ b/Base de Datos/COMPUTACIÓN 201835  Semestral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTO_SCRUM_IS_II\LoboServicesFCC\Base de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D8253B-5B05-4122-A80C-EA7FD9083CBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47C573F-8E59-4221-9034-2158616B3B25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="semestral" sheetId="6" r:id="rId1"/>
@@ -21288,7 +21288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82DFC6E-E826-4178-AF7A-7971C314C365}">
   <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -21325,8 +21325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03379B5D-3AFA-44CA-B431-D65A6289F440}">
   <dimension ref="B2:J75"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22970,7 +22970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B65" s="2">
         <v>63</v>
       </c>
@@ -22989,8 +22989,14 @@
       <c r="G65" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I65" s="2">
+        <v>42</v>
+      </c>
+      <c r="J65" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B66" s="2">
         <v>64</v>
       </c>
@@ -23009,8 +23015,14 @@
       <c r="G66" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I66" s="2">
+        <v>56</v>
+      </c>
+      <c r="J66" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B67" s="2">
         <v>65</v>
       </c>
@@ -23029,8 +23041,14 @@
       <c r="G67" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I67" s="2">
+        <v>5</v>
+      </c>
+      <c r="J67" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B68" s="2">
         <v>66</v>
       </c>
@@ -23050,7 +23068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B69" s="2">
         <v>67</v>
       </c>
@@ -23070,7 +23088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B70" s="2">
         <v>68</v>
       </c>
@@ -23090,7 +23108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B71" s="2">
         <v>69</v>
       </c>
@@ -23110,7 +23128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B72" s="2">
         <v>70</v>
       </c>
@@ -23130,7 +23148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B73" s="2">
         <v>71</v>
       </c>
@@ -23150,7 +23168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B74" s="2">
         <v>72</v>
       </c>
@@ -23170,7 +23188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B75" s="2">
         <v>73</v>
       </c>

</xml_diff>